<commit_message>
Task-List done    (Issue, not possible to read all tasks with skills and parameters!) Order: "I feel lucky", "1-click-order" Adaptions in SB Admin V2 Added: Debugging Functions
</commit_message>
<xml_diff>
--- a/misc/Eventlist.xlsx
+++ b/misc/Eventlist.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>IO.emit() - Events</t>
   </si>
@@ -51,13 +51,22 @@
   </si>
   <si>
     <t>sbadmin.jade / +dropdown-time()</t>
+  </si>
+  <si>
+    <t>bgOpcuaConnection</t>
+  </si>
+  <si>
+    <t>1 / 0</t>
+  </si>
+  <si>
+    <t>backgroundServices.js</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,6 +78,13 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,7 +120,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -115,19 +131,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -150,13 +190,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:D11" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:D11" totalsRowShown="0" headerRowDxfId="5" dataDxfId="0" tableBorderDxfId="6">
   <autoFilter ref="A2:D11"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="EventName"/>
-    <tableColumn id="2" name="Data" dataDxfId="1"/>
-    <tableColumn id="3" name="emitted from"/>
-    <tableColumn id="4" name="emitted to"/>
+    <tableColumn id="1" name="EventName" dataDxfId="4"/>
+    <tableColumn id="2" name="Data" dataDxfId="3"/>
+    <tableColumn id="3" name="emitted from" dataDxfId="2"/>
+    <tableColumn id="4" name="emitted to" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -428,7 +468,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,27 +502,73 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
     <row r="12" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>